<commit_message>
prueba para visual iphone
</commit_message>
<xml_diff>
--- a/public/productos.xlsx
+++ b/public/productos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jamil\j-app\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA9F776-70F4-4B2B-9FF6-4F4BCEC88EAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7237C04D-CB1F-4E8E-A7CF-AA74C571A9D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{55BB4BDA-9EF4-45BB-8459-F2BE00004C01}"/>
+    <workbookView xWindow="735" yWindow="735" windowWidth="28800" windowHeight="15345" xr2:uid="{55BB4BDA-9EF4-45BB-8459-F2BE00004C01}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -6958,7 +6958,7 @@
   <dimension ref="A1:I1932"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1932" sqref="E2:E1932"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>